<commit_message>
Added some poisson loo numbers
</commit_message>
<xml_diff>
--- a/LOO_CV_numbers.xlsx
+++ b/LOO_CV_numbers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzraw\OneDrive\Documents\R\Spatial_COVID_modelling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzraw\OneDrive - Imperial College London\Documents\R\spatial_uk_covid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222A3817-4E99-40C9-B0EB-0EB97203FB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BBB52C-C150-46F3-87C0-C95BE23942F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="3645" windowWidth="26970" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="360" windowWidth="21600" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,12 +220,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -249,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -258,6 +264,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,6 +1231,18 @@
       <c r="C33" t="s">
         <v>51</v>
       </c>
+      <c r="D33" s="8">
+        <v>0.67</v>
+      </c>
+      <c r="E33" s="2">
+        <v>-354064</v>
+      </c>
+      <c r="F33" s="2">
+        <v>48022</v>
+      </c>
+      <c r="G33" s="2">
+        <v>708129</v>
+      </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -1250,7 +1269,21 @@
       <c r="C35" t="s">
         <v>54</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="D35" s="1">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="E35" s="2">
+        <v>-355560</v>
+      </c>
+      <c r="F35" s="2">
+        <v>14532</v>
+      </c>
+      <c r="G35" s="2">
+        <v>711120</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
@@ -1776,13 +1809,13 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
         <color theme="9" tint="0.59999389629810485"/>
-        <color theme="5" tint="0.59999389629810485"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1796,13 +1829,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color theme="9" tint="0.59999389629810485"/>
         <color theme="5" tint="0.59999389629810485"/>
-        <color theme="9" tint="0.59999389629810485"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>